<commit_message>
Add data provider for testLogInWithInvalidInput test
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A6C4C9-8BC0-4808-BEC7-FAD91032B517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculator" sheetId="2" r:id="rId2"/>
-    <sheet name="Data" sheetId="3" r:id="rId3"/>
+    <sheet name="LoginData" sheetId="4" r:id="rId2"/>
+    <sheet name="Calculator" sheetId="2" r:id="rId3"/>
+    <sheet name="Data" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Execute</t>
   </si>
@@ -221,13 +221,52 @@
   </si>
   <si>
     <t>8GB RAM</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>123457687AAAsad</t>
+  </si>
+  <si>
+    <t>inputWithInvalidEmail</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. 'invalidEmail' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>testEmail@</t>
+  </si>
+  <si>
+    <t>Please enter a part following '@'. 'testEmail@' is incomplete.</t>
+  </si>
+  <si>
+    <t>inputWithIncompleteEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @gmail.com</t>
+  </si>
+  <si>
+    <t>inputWithIncompleteEmail2</t>
+  </si>
+  <si>
+    <t>Please enter a part followed by '@'. '@gmail.com' is incomplete.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +309,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -300,11 +353,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,10 +380,20 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{54382045-ACAB-4016-8E48-6E3B48DC3618}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -353,9 +417,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +457,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -428,23 +492,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -480,26 +527,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -672,10 +702,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -802,7 +832,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -889,8 +1012,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159BBBDB-2C19-4029-8CF8-DF830F70E1A1}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>